<commit_message>
新增deleteCloudDiskSnap.py getInstanceSnapDetails.py putCloudDiskSnap.py restoreCloudDiskSnap.py searchCloudDiskSnap.py 脚本
</commit_message>
<xml_diff>
--- a/datafiles/snapsMagData.xlsx
+++ b/datafiles/snapsMagData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9300" firstSheet="2" activeTab="7"/>
+    <workbookView windowWidth="23040" windowHeight="9300" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="getPoolSnapList" sheetId="30" r:id="rId1"/>
@@ -15,13 +15,18 @@
     <sheet name="restoreInstanceSnap" sheetId="35" r:id="rId6"/>
     <sheet name="deleteInstanceSnap" sheetId="36" r:id="rId7"/>
     <sheet name="searchInstanceSnap" sheetId="37" r:id="rId8"/>
+    <sheet name="getInstanceSnapDetails" sheetId="38" r:id="rId9"/>
+    <sheet name="restoreCloudDiskSnap" sheetId="39" r:id="rId10"/>
+    <sheet name="deleteCloudDiskSnap" sheetId="40" r:id="rId11"/>
+    <sheet name="putCloudDiskSnap" sheetId="41" r:id="rId12"/>
+    <sheet name="searchCloudDiskSnap" sheetId="42" r:id="rId13"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="99">
   <si>
     <t>test_num</t>
   </si>
@@ -183,10 +188,234 @@
     <t>查询云组件快照-缺少token</t>
   </si>
   <si>
+    <t>{
+    "pag":"1",
+    "size":"10",
+    "search_field":"snapshot_name",
+    "search":"snap"
+}</t>
+  </si>
+  <si>
+    <t>查询云组件快照-成功</t>
+  </si>
+  <si>
+    <t>查询云组件快照详情-缺少token</t>
+  </si>
+  <si>
     <t>{}</t>
   </si>
   <si>
-    <t>查询云组件快照-成功</t>
+    <t>查询云组件快照详情-成功</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>回滚云硬盘快照-缺少token</t>
+  </si>
+  <si>
+    <t>回滚云硬盘快照-project_id为空</t>
+  </si>
+  <si>
+    <t>{
+    "project_id":"",
+    "project_name":"HJp0_hash"
+}</t>
+  </si>
+  <si>
+    <t>服务端project_id和project_name非必填</t>
+  </si>
+  <si>
+    <t>回滚云硬盘快照-project_name为空</t>
+  </si>
+  <si>
+    <t>{
+    "project_id":"c732c22666064375904c357bbecfeb1a",
+    "project_name":""
+}</t>
+  </si>
+  <si>
+    <t>回滚云硬盘快照-成功</t>
+  </si>
+  <si>
+    <t>删除云硬盘快照-缺少token</t>
+  </si>
+  <si>
+    <t>{
+    "ids":[
+        "f9cfdfb4-6ce7-4530-9f78-d435f58d521c"
+    ],
+    "project_id":"c732c22666064375904c357bbecfeb1a",
+    "project_name":"HJp0_hash"
+}</t>
+  </si>
+  <si>
+    <t>删除云硬盘快照-云硬盘快照ids为空</t>
+  </si>
+  <si>
+    <t>{
+    "ids":[],
+    "project_id":"c732c22666064375904c357bbecfeb1a",
+    "project_name":"HJp0_hash"
+}</t>
+  </si>
+  <si>
+    <t>{'ids': ['Ensure this field has at least 1 elements.']}</t>
+  </si>
+  <si>
+    <t>删除云硬盘快照-project_id为空</t>
+  </si>
+  <si>
+    <t>{
+    "ids":[
+        "f9cfdfb4-6ce7-4530-9f78-d435f58d521c"
+    ],
+    "project_id":"",
+    "project_name":"HJp0_hash"
+}</t>
+  </si>
+  <si>
+    <t>删除云硬盘快照-project_name为空</t>
+  </si>
+  <si>
+    <t>{
+    "ids":[
+        "f9cfdfb4-6ce7-4530-9f78-d435f58d521c"
+    ],
+    "project_id":"c732c22666064375904c357bbecfeb1a",
+    "project_name":""
+}</t>
+  </si>
+  <si>
+    <t>删除云硬盘快照-云硬盘快照删除成功</t>
+  </si>
+  <si>
+    <t>{
+    "ids":[
+        "f9cfdfb4-6ce9-4530-9aa8-d435f58da21c"
+    ],
+    "project_id":"c732c22666064375904c357bbecfeb1a",
+    "project_name":"HJp0_hash"
+}</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>删除云硬盘快照-云硬盘快照ids不存在</t>
+  </si>
+  <si>
+    <t>云硬盘快照不存在</t>
+  </si>
+  <si>
+    <t>编辑云硬盘快照-缺少token</t>
+  </si>
+  <si>
+    <t>{
+    "name":"cdSanp2"
+}</t>
+  </si>
+  <si>
+    <t>编辑云硬盘快照-云硬盘id不存在</t>
+  </si>
+  <si>
+    <t>编辑云硬盘快照-name为空</t>
+  </si>
+  <si>
+    <t>{
+    "name":""
+}</t>
+  </si>
+  <si>
+    <t>{'name': ['该字段不能为空。']}</t>
+  </si>
+  <si>
+    <t>编辑云硬盘快照-name大于32个字符</t>
+  </si>
+  <si>
+    <t>{
+    "name":"aaaaabbbbbaaaaabbbbbaaaaabbbbb12345"
+}</t>
+  </si>
+  <si>
+    <t>快照名称过长</t>
+  </si>
+  <si>
+    <t>编辑云硬盘快照-name为中文</t>
+  </si>
+  <si>
+    <t>{
+    "name":"中文名称云硬盘快照"
+}</t>
+  </si>
+  <si>
+    <t>快照名称只能输入数字、字母、-、_, 只允许以英文开头</t>
+  </si>
+  <si>
+    <t>编辑云硬盘快照-name为特殊字符</t>
+  </si>
+  <si>
+    <t>{
+    "name":"……&amp;……&amp;%……%"
+}</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>编辑云硬盘快照-name以数字开头</t>
+  </si>
+  <si>
+    <t>{
+    "name":"11112222"
+}</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>编辑云硬盘快照-name以下划线开头</t>
+  </si>
+  <si>
+    <t>{
+    "name":"__asdada"
+}</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>编辑云硬盘快照-name以短横线开头</t>
+  </si>
+  <si>
+    <t>{
+    "name":"--asdada"
+}</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>编辑云硬盘快照-合规name编辑成功</t>
+  </si>
+  <si>
+    <t>{
+    "name":"SnapNameUp-1_success"
+}</t>
+  </si>
+  <si>
+    <t>搜索云硬盘快照-缺少token</t>
+  </si>
+  <si>
+    <t>{
+    "pag":"1",
+    "size":"10",
+    "search_field":"name",
+    "search":"d"
+}</t>
+  </si>
+  <si>
+    <t>搜索云硬盘快照</t>
   </si>
 </sst>
 </file>
@@ -194,10 +423,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -228,6 +457,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -235,8 +494,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -250,38 +525,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -297,46 +559,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -344,19 +574,18 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -379,25 +608,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,151 +776,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -607,6 +836,30 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -617,30 +870,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -674,8 +903,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -685,10 +914,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -697,135 +926,135 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -833,7 +1062,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="50" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -848,6 +1077,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="50" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="50" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1272,6 +1504,646 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>
+  <cols>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="56.75" customWidth="1"/>
+    <col min="5" max="5" width="18.125" customWidth="1"/>
+    <col min="7" max="7" width="39.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" ht="27" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1005</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" ht="54" spans="1:7">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" ht="54" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="94.5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6" outlineLevelCol="6"/>
+  <cols>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="47.875" customWidth="1"/>
+    <col min="5" max="5" width="29.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" ht="121.5" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1005</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" ht="94.5" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1001</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" ht="94.5" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="121.5" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" s="2" customFormat="1" ht="121.5" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6"/>
+    </row>
+    <row r="7" s="2" customFormat="1" ht="121.5" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="2">
+        <v>214006</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <cols>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="47.875" customWidth="1"/>
+    <col min="5" max="5" width="29.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" ht="40.5" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1005</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="40.5" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="2">
+        <v>214006</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="2" customFormat="1" ht="40.5" spans="1:6">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1001</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4"/>
+    </row>
+    <row r="5" s="2" customFormat="1" ht="54" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="2">
+        <v>214022</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5"/>
+    </row>
+    <row r="6" s="2" customFormat="1" ht="40.5" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="2">
+        <v>214020</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6"/>
+    </row>
+    <row r="7" s="2" customFormat="1" ht="40.5" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="2">
+        <v>214020</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7"/>
+    </row>
+    <row r="8" s="2" customFormat="1" ht="40.5" spans="1:6">
+      <c r="A8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="2">
+        <v>214020</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8"/>
+    </row>
+    <row r="9" ht="40.5" spans="1:5">
+      <c r="A9" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" s="2">
+        <v>214020</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" ht="40.5" spans="1:5">
+      <c r="A10" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="2">
+        <v>214020</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" ht="40.5" spans="1:4">
+      <c r="A11" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <cols>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="47.875" customWidth="1"/>
+    <col min="5" max="5" width="29.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" s="2" customFormat="1" ht="81" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1005</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="81" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" s="2" customFormat="1" spans="1:6">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4"/>
+    </row>
+    <row r="5" s="2" customFormat="1" spans="1:6">
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5"/>
+    </row>
+    <row r="6" s="2" customFormat="1" spans="1:6">
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6"/>
+    </row>
+    <row r="7" s="2" customFormat="1" spans="1:6">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7"/>
+    </row>
+    <row r="8" s="2" customFormat="1" spans="1:6">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" customFormat="1" spans="1:3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
@@ -1626,7 +2498,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A1" sqref="$A1:$XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="5"/>
@@ -1828,7 +2700,6 @@
       <c r="D3" s="2">
         <v>0</v>
       </c>
-      <c r="E3" s="2"/>
       <c r="F3"/>
     </row>
   </sheetData>
@@ -1843,7 +2714,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="5"/>
@@ -1873,15 +2744,92 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2" s="2" customFormat="1" ht="81" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1005</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" s="2" customFormat="1" ht="81" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2" outlineLevelCol="5"/>
+  <cols>
+    <col min="2" max="2" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="47.875" customWidth="1"/>
+    <col min="5" max="5" width="29.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2" s="2" customFormat="1" spans="1:6">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2">
         <v>1005</v>
@@ -1898,10 +2846,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>

</xml_diff>